<commit_message>
Update install and others
</commit_message>
<xml_diff>
--- a/Examples/ParticipationAnalysis/ModalConfig_UserData.xlsx
+++ b/Examples/ParticipationAnalysis/ModalConfig_UserData.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Git\Simplex-Power-Systems\Examples\ParticipationAnalysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\Examples\ParticipationAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56842C30-8711-4EDE-A7F5-9B040EA208EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDFF8024-9ED6-455C-BE8E-25D4464FBCE3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{AB139ACC-3F1C-4B61-BC2D-96F2B1E0C6D8}"/>
+    <workbookView xWindow="0" yWindow="2820" windowWidth="14400" windowHeight="7380" activeTab="2" xr2:uid="{AB139ACC-3F1C-4B61-BC2D-96F2B1E0C6D8}"/>
   </bookViews>
   <sheets>
-    <sheet name="State-PF" sheetId="18" r:id="rId1"/>
-    <sheet name="Impedance-PF" sheetId="19" r:id="rId2"/>
-    <sheet name="Enabling" sheetId="20" r:id="rId3"/>
+    <sheet name="State-PF" sheetId="33" r:id="rId1"/>
+    <sheet name="Impedance-PF" sheetId="34" r:id="rId2"/>
+    <sheet name="Enabling" sheetId="35" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -494,12 +494,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -838,26 +845,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F0240F0-8481-4178-85BF-448C2DBB5348}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{650F62C6-06C0-4F27-A4F6-31A85150FF31}">
   <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:G71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -877,7 +884,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -897,7 +904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -914,7 +921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
         <v>12</v>
       </c>
@@ -931,7 +938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
         <v>14</v>
       </c>
@@ -948,7 +955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
         <v>16</v>
       </c>
@@ -965,7 +972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -985,7 +992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -1002,7 +1009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
         <v>12</v>
       </c>
@@ -1019,7 +1026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
         <v>14</v>
       </c>
@@ -1036,7 +1043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
         <v>16</v>
       </c>
@@ -1053,7 +1060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1073,7 +1080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B18" t="s">
         <v>10</v>
       </c>
@@ -1090,7 +1097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B19" t="s">
         <v>12</v>
       </c>
@@ -1107,7 +1114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B20" t="s">
         <v>14</v>
       </c>
@@ -1124,7 +1131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B21" t="s">
         <v>16</v>
       </c>
@@ -1141,7 +1148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -1161,7 +1168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
         <v>10</v>
       </c>
@@ -1178,7 +1185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
         <v>12</v>
       </c>
@@ -1195,7 +1202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B25" t="s">
         <v>48</v>
       </c>
@@ -1212,7 +1219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B26" t="s">
         <v>51</v>
       </c>
@@ -1229,7 +1236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B27" t="s">
         <v>54</v>
       </c>
@@ -1246,7 +1253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B28" t="s">
         <v>14</v>
       </c>
@@ -1263,7 +1270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
         <v>16</v>
       </c>
@@ -1280,7 +1287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B30" t="s">
         <v>60</v>
       </c>
@@ -1297,7 +1304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B31" t="s">
         <v>63</v>
       </c>
@@ -1314,7 +1321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>66</v>
       </c>
@@ -1334,7 +1341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B33" t="s">
         <v>70</v>
       </c>
@@ -1351,7 +1358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B34" t="s">
         <v>73</v>
       </c>
@@ -1368,7 +1375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B35" t="s">
         <v>76</v>
       </c>
@@ -1385,7 +1392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B36" t="s">
         <v>79</v>
       </c>
@@ -1402,7 +1409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B37" t="s">
         <v>81</v>
       </c>
@@ -1419,7 +1426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
         <v>73</v>
       </c>
@@ -1436,7 +1443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B39" t="s">
         <v>76</v>
       </c>
@@ -1453,7 +1460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B40" t="s">
         <v>79</v>
       </c>
@@ -1470,7 +1477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B41" t="s">
         <v>81</v>
       </c>
@@ -1487,7 +1494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B42" t="s">
         <v>73</v>
       </c>
@@ -1504,7 +1511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B43" t="s">
         <v>76</v>
       </c>
@@ -1521,7 +1528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B44" t="s">
         <v>73</v>
       </c>
@@ -1538,7 +1545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B45" t="s">
         <v>76</v>
       </c>
@@ -1555,7 +1562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B46" t="s">
         <v>97</v>
       </c>
@@ -1572,7 +1579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B47" t="s">
         <v>100</v>
       </c>
@@ -1589,7 +1596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B48" t="s">
         <v>103</v>
       </c>
@@ -1606,7 +1613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B49" t="s">
         <v>105</v>
       </c>
@@ -1623,7 +1630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B50" t="s">
         <v>103</v>
       </c>
@@ -1640,7 +1647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B51" t="s">
         <v>105</v>
       </c>
@@ -1657,7 +1664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B52" t="s">
         <v>79</v>
       </c>
@@ -1674,7 +1681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B53" t="s">
         <v>81</v>
       </c>
@@ -1691,7 +1698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B54" t="s">
         <v>103</v>
       </c>
@@ -1708,7 +1715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B55" t="s">
         <v>105</v>
       </c>
@@ -1725,7 +1732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B56" t="s">
         <v>79</v>
       </c>
@@ -1742,7 +1749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B57" t="s">
         <v>81</v>
       </c>
@@ -1759,7 +1766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B58" t="s">
         <v>103</v>
       </c>
@@ -1776,7 +1783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B59" t="s">
         <v>105</v>
       </c>
@@ -1793,7 +1800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B60" t="s">
         <v>117</v>
       </c>
@@ -1810,7 +1817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B61" t="s">
         <v>119</v>
       </c>
@@ -1827,7 +1834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B62" t="s">
         <v>121</v>
       </c>
@@ -1844,7 +1851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B63" t="s">
         <v>123</v>
       </c>
@@ -1861,7 +1868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B64" t="s">
         <v>121</v>
       </c>
@@ -1878,7 +1885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B65" t="s">
         <v>123</v>
       </c>
@@ -1895,7 +1902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B66" t="s">
         <v>121</v>
       </c>
@@ -1912,7 +1919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B67" t="s">
         <v>123</v>
       </c>
@@ -1929,7 +1936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B68" t="s">
         <v>121</v>
       </c>
@@ -1946,7 +1953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B69" t="s">
         <v>123</v>
       </c>
@@ -1963,7 +1970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B70" t="s">
         <v>131</v>
       </c>
@@ -1980,7 +1987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B71" t="s">
         <v>133</v>
       </c>
@@ -1998,31 +2005,33 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77990D4D-087C-4EFB-9BF8-FC32D7EE6F25}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E166FDB-7F7C-4809-882A-350B9959AA13}">
   <dimension ref="A1:L72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:L72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>136</v>
       </c>
@@ -2036,7 +2045,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -2065,7 +2074,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2094,7 +2103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -2123,7 +2132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -2152,7 +2161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -2181,7 +2190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="G12" t="s">
         <v>17</v>
       </c>
@@ -2192,7 +2201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="G13" t="s">
         <v>20</v>
       </c>
@@ -2203,7 +2212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="G14" t="s">
         <v>22</v>
       </c>
@@ -2214,7 +2223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
       <c r="G15" t="s">
         <v>24</v>
       </c>
@@ -2225,7 +2234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
       <c r="G16" t="s">
         <v>26</v>
       </c>
@@ -2236,7 +2245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G17" t="s">
         <v>28</v>
       </c>
@@ -2247,7 +2256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G18" t="s">
         <v>31</v>
       </c>
@@ -2258,7 +2267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G19" t="s">
         <v>33</v>
       </c>
@@ -2269,7 +2278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G20" t="s">
         <v>35</v>
       </c>
@@ -2280,7 +2289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G21" t="s">
         <v>37</v>
       </c>
@@ -2291,7 +2300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G22" t="s">
         <v>39</v>
       </c>
@@ -2302,7 +2311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G23" t="s">
         <v>42</v>
       </c>
@@ -2313,7 +2322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G24" t="s">
         <v>44</v>
       </c>
@@ -2324,7 +2333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G25" t="s">
         <v>46</v>
       </c>
@@ -2335,7 +2344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G26" t="s">
         <v>49</v>
       </c>
@@ -2346,7 +2355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G27" t="s">
         <v>52</v>
       </c>
@@ -2357,7 +2366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G28" t="s">
         <v>55</v>
       </c>
@@ -2368,7 +2377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G29" t="s">
         <v>56</v>
       </c>
@@ -2379,7 +2388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G30" t="s">
         <v>58</v>
       </c>
@@ -2390,7 +2399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G31" t="s">
         <v>61</v>
       </c>
@@ -2401,7 +2410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G32" t="s">
         <v>64</v>
       </c>
@@ -2412,7 +2421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G33" t="s">
         <v>68</v>
       </c>
@@ -2423,7 +2432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G34" t="s">
         <v>71</v>
       </c>
@@ -2434,7 +2443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G35" t="s">
         <v>74</v>
       </c>
@@ -2445,7 +2454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G36" t="s">
         <v>77</v>
       </c>
@@ -2456,7 +2465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G37" t="s">
         <v>80</v>
       </c>
@@ -2467,7 +2476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G38" t="s">
         <v>82</v>
       </c>
@@ -2478,7 +2487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G39" t="s">
         <v>84</v>
       </c>
@@ -2489,7 +2498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G40" t="s">
         <v>86</v>
       </c>
@@ -2500,7 +2509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G41" t="s">
         <v>88</v>
       </c>
@@ -2511,7 +2520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G42" t="s">
         <v>90</v>
       </c>
@@ -2522,7 +2531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G43" t="s">
         <v>91</v>
       </c>
@@ -2533,7 +2542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G44" t="s">
         <v>93</v>
       </c>
@@ -2544,7 +2553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G45" t="s">
         <v>95</v>
       </c>
@@ -2555,7 +2564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G46" t="s">
         <v>96</v>
       </c>
@@ -2566,7 +2575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G47" t="s">
         <v>98</v>
       </c>
@@ -2577,7 +2586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G48" t="s">
         <v>101</v>
       </c>
@@ -2588,7 +2597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G49" t="s">
         <v>104</v>
       </c>
@@ -2599,7 +2608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G50" t="s">
         <v>106</v>
       </c>
@@ -2610,7 +2619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G51" t="s">
         <v>107</v>
       </c>
@@ -2621,7 +2630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G52" t="s">
         <v>108</v>
       </c>
@@ -2632,7 +2641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G53" t="s">
         <v>109</v>
       </c>
@@ -2643,7 +2652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G54" t="s">
         <v>110</v>
       </c>
@@ -2654,7 +2663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G55" t="s">
         <v>111</v>
       </c>
@@ -2665,7 +2674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G56" t="s">
         <v>112</v>
       </c>
@@ -2676,7 +2685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G57" t="s">
         <v>113</v>
       </c>
@@ -2687,7 +2696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G58" t="s">
         <v>114</v>
       </c>
@@ -2698,7 +2707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G59" t="s">
         <v>115</v>
       </c>
@@ -2709,7 +2718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G60" t="s">
         <v>116</v>
       </c>
@@ -2720,7 +2729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G61" t="s">
         <v>118</v>
       </c>
@@ -2731,7 +2740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G62" t="s">
         <v>120</v>
       </c>
@@ -2742,7 +2751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G63" t="s">
         <v>122</v>
       </c>
@@ -2753,7 +2762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G64" t="s">
         <v>124</v>
       </c>
@@ -2764,7 +2773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G65" t="s">
         <v>125</v>
       </c>
@@ -2775,7 +2784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G66" t="s">
         <v>126</v>
       </c>
@@ -2786,7 +2795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G67" t="s">
         <v>127</v>
       </c>
@@ -2797,7 +2806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G68" t="s">
         <v>128</v>
       </c>
@@ -2808,7 +2817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G69" t="s">
         <v>129</v>
       </c>
@@ -2819,7 +2828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G70" t="s">
         <v>130</v>
       </c>
@@ -2830,7 +2839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G71" t="s">
         <v>132</v>
       </c>
@@ -2841,7 +2850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="7:9" x14ac:dyDescent="0.4">
       <c r="G72" t="s">
         <v>134</v>
       </c>
@@ -2853,31 +2862,32 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3454F0CF-4216-471F-928F-55C163C82ECE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49AD8F46-ED6F-4303-8A8F-1839F22EE618}">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>146</v>
       </c>
@@ -2885,7 +2895,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>147</v>
       </c>
@@ -2893,7 +2903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>148</v>
       </c>
@@ -2901,7 +2911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>149</v>
       </c>
@@ -2909,7 +2919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>150</v>
       </c>
@@ -2918,6 +2928,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>